<commit_message>
Update burndown with my details
</commit_message>
<xml_diff>
--- a/ProjectPlanning_Current.xlsx
+++ b/ProjectPlanning_Current.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kamakazi\Documents\MAD\MAD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\AndroidStudioProjects\MAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5940" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5940" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="BurndownChartTemplate" sheetId="3" r:id="rId1"/>
@@ -1221,26 +1221,6 @@
     <xf numFmtId="0" fontId="10" fillId="14" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1250,7 +1230,78 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1271,60 +1322,48 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1354,45 +1393,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -2471,7 +2471,7 @@
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>10</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5225,11 +5225,11 @@
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="59"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="54"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="1"/>
@@ -5476,14 +5476,14 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="54" t="s">
+      <c r="D11" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
       <c r="J11" s="1"/>
       <c r="K11" s="20" t="s">
         <v>33</v>
@@ -5518,10 +5518,10 @@
     </row>
     <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="61"/>
+      <c r="C13" s="56"/>
       <c r="D13" s="17" t="s">
         <v>0</v>
       </c>
@@ -5548,10 +5548,10 @@
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="53"/>
+      <c r="C14" s="58"/>
       <c r="D14" s="18" t="s">
         <v>6</v>
       </c>
@@ -5578,10 +5578,10 @@
     </row>
     <row r="15" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="53"/>
+      <c r="C15" s="58"/>
       <c r="D15" s="18" t="s">
         <v>7</v>
       </c>
@@ -5608,10 +5608,10 @@
     </row>
     <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="52" t="s">
+      <c r="B16" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="53"/>
+      <c r="C16" s="58"/>
       <c r="D16" s="18" t="s">
         <v>8</v>
       </c>
@@ -5638,10 +5638,10 @@
     </row>
     <row r="17" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="53"/>
+      <c r="C17" s="58"/>
       <c r="D17" s="18" t="s">
         <v>9</v>
       </c>
@@ -5668,10 +5668,10 @@
     </row>
     <row r="18" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="52" t="s">
+      <c r="B18" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="53"/>
+      <c r="C18" s="58"/>
       <c r="D18" s="18" t="s">
         <v>10</v>
       </c>
@@ -5698,10 +5698,10 @@
     </row>
     <row r="19" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="52" t="s">
+      <c r="B19" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="53"/>
+      <c r="C19" s="58"/>
       <c r="D19" s="18" t="s">
         <v>11</v>
       </c>
@@ -5728,10 +5728,10 @@
     </row>
     <row r="20" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="52" t="s">
+      <c r="B20" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="53"/>
+      <c r="C20" s="58"/>
       <c r="D20" s="18" t="s">
         <v>12</v>
       </c>
@@ -5758,10 +5758,10 @@
     </row>
     <row r="21" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="52" t="s">
+      <c r="B21" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="53"/>
+      <c r="C21" s="58"/>
       <c r="D21" s="18" t="s">
         <v>13</v>
       </c>
@@ -5788,10 +5788,10 @@
     </row>
     <row r="22" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="53"/>
+      <c r="C22" s="58"/>
       <c r="D22" s="18" t="s">
         <v>14</v>
       </c>
@@ -5818,10 +5818,10 @@
     </row>
     <row r="23" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="53"/>
+      <c r="C23" s="58"/>
       <c r="D23" s="18" t="s">
         <v>15</v>
       </c>
@@ -5848,10 +5848,10 @@
     </row>
     <row r="24" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="52" t="s">
+      <c r="B24" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="53"/>
+      <c r="C24" s="58"/>
       <c r="D24" s="18" t="s">
         <v>16</v>
       </c>
@@ -5878,10 +5878,10 @@
     </row>
     <row r="25" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="52" t="s">
+      <c r="B25" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="53"/>
+      <c r="C25" s="58"/>
       <c r="D25" s="18" t="s">
         <v>17</v>
       </c>
@@ -5908,10 +5908,10 @@
     </row>
     <row r="26" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="52" t="s">
+      <c r="B26" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="53"/>
+      <c r="C26" s="58"/>
       <c r="D26" s="18" t="s">
         <v>18</v>
       </c>
@@ -5938,11 +5938,11 @@
     </row>
     <row r="27" spans="1:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
       <c r="E27" s="19">
         <f>SUM(E14:E26)</f>
         <v>40</v>
@@ -5972,11 +5972,11 @@
     </row>
     <row r="28" spans="1:20" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="55" t="s">
+      <c r="B28" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
       <c r="E28" s="19">
         <f>SUM(E14:E26)</f>
         <v>40</v>
@@ -6067,11 +6067,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="D11:I11"/>
@@ -6085,6 +6080,11 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6281,7 +6281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
@@ -6297,11 +6297,11 @@
     <row r="1" spans="2:9" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="59"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="54"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
@@ -6430,18 +6430,18 @@
       <c r="G10" s="2"/>
     </row>
     <row r="15" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="77" t="s">
+      <c r="D15" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
     </row>
     <row r="16" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="77"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
       <c r="H16" t="s">
         <v>70</v>
       </c>
@@ -6451,15 +6451,15 @@
     </row>
     <row r="17" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="3:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="63" t="s">
+      <c r="C18" s="80" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="64"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="66" t="s">
+      <c r="D18" s="81"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="67"/>
+      <c r="G18" s="84"/>
       <c r="H18" s="48" t="s">
         <v>1</v>
       </c>
@@ -6474,15 +6474,15 @@
       </c>
     </row>
     <row r="19" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C19" s="68" t="s">
+      <c r="C19" s="85" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="69"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="74" t="s">
+      <c r="D19" s="86"/>
+      <c r="E19" s="87"/>
+      <c r="F19" s="88" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="74"/>
+      <c r="G19" s="88"/>
       <c r="H19" s="50">
         <v>2</v>
       </c>
@@ -6497,13 +6497,13 @@
       </c>
     </row>
     <row r="20" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C20" s="71"/>
-      <c r="D20" s="72"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="62" t="s">
+      <c r="C20" s="69"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="G20" s="62"/>
+      <c r="G20" s="77"/>
       <c r="H20" s="36">
         <v>4</v>
       </c>
@@ -6518,15 +6518,15 @@
       </c>
     </row>
     <row r="21" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C21" s="85" t="s">
+      <c r="C21" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="62" t="s">
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="G21" s="62"/>
+      <c r="G21" s="77"/>
       <c r="H21" s="36">
         <v>1</v>
       </c>
@@ -6541,13 +6541,13 @@
       </c>
     </row>
     <row r="22" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C22" s="85"/>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="62" t="s">
+      <c r="C22" s="75"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="G22" s="62"/>
+      <c r="G22" s="77"/>
       <c r="H22" s="36">
         <v>2</v>
       </c>
@@ -6562,9 +6562,9 @@
       </c>
     </row>
     <row r="23" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C23" s="85"/>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="76"/>
       <c r="F23" s="47" t="s">
         <v>75</v>
       </c>
@@ -6583,81 +6583,81 @@
       </c>
     </row>
     <row r="24" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C24" s="79" t="s">
+      <c r="C24" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="80"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="77"/>
+      <c r="G24" s="77"/>
       <c r="H24" s="36"/>
       <c r="I24" s="36"/>
       <c r="J24" s="36"/>
       <c r="K24" s="37"/>
     </row>
     <row r="25" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C25" s="71"/>
-      <c r="D25" s="72"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="77"/>
       <c r="H25" s="36"/>
       <c r="I25" s="36"/>
       <c r="J25" s="36"/>
       <c r="K25" s="37"/>
     </row>
     <row r="26" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C26" s="82"/>
-      <c r="D26" s="83"/>
-      <c r="E26" s="84"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="77"/>
       <c r="H26" s="36"/>
       <c r="I26" s="36"/>
       <c r="J26" s="36"/>
       <c r="K26" s="37"/>
     </row>
     <row r="27" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C27" s="85"/>
-      <c r="D27" s="86"/>
-      <c r="E27" s="86"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="77"/>
       <c r="H27" s="36"/>
       <c r="I27" s="36"/>
       <c r="J27" s="36"/>
       <c r="K27" s="37"/>
     </row>
     <row r="28" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C28" s="85"/>
-      <c r="D28" s="86"/>
-      <c r="E28" s="86"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="62"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="76"/>
+      <c r="F28" s="77"/>
+      <c r="G28" s="77"/>
       <c r="H28" s="36"/>
       <c r="I28" s="36"/>
       <c r="J28" s="36"/>
       <c r="K28" s="37"/>
     </row>
     <row r="29" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C29" s="85"/>
-      <c r="D29" s="86"/>
-      <c r="E29" s="86"/>
-      <c r="F29" s="62"/>
-      <c r="G29" s="62"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="77"/>
       <c r="H29" s="36"/>
       <c r="I29" s="36"/>
       <c r="J29" s="36"/>
       <c r="K29" s="37"/>
     </row>
     <row r="30" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C30" s="87" t="s">
+      <c r="C30" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="88"/>
-      <c r="E30" s="88"/>
-      <c r="F30" s="88"/>
-      <c r="G30" s="88"/>
+      <c r="D30" s="79"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
       <c r="H30" s="38">
         <f>SUM(H19:H29)</f>
         <v>11</v>
@@ -6676,13 +6676,13 @@
       </c>
     </row>
     <row r="31" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="75" t="s">
+      <c r="C31" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="D31" s="76"/>
-      <c r="E31" s="76"/>
-      <c r="F31" s="76"/>
-      <c r="G31" s="76"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="63"/>
+      <c r="G31" s="63"/>
       <c r="H31" s="40">
         <f>SUM(H19:H29)</f>
         <v>11</v>
@@ -6702,6 +6702,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="C19:E20"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
     <mergeCell ref="C31:G31"/>
     <mergeCell ref="D15:G16"/>
     <mergeCell ref="C24:E26"/>
@@ -6716,14 +6724,6 @@
     <mergeCell ref="F27:G27"/>
     <mergeCell ref="C21:E23"/>
     <mergeCell ref="F21:G21"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="C19:E20"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -6735,8 +6735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J33"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6751,11 +6751,11 @@
     <row r="1" spans="2:8" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="59"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="54"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
@@ -6843,11 +6843,11 @@
         <v>6</v>
       </c>
       <c r="E8" s="7">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F8" s="11">
         <f>SUM(C8:E8)</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -6865,7 +6865,7 @@
       </c>
       <c r="E9" s="14">
         <f>SUM(E5:E8)</f>
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -6876,7 +6876,7 @@
       </c>
       <c r="C10" s="16">
         <f>SUM(C9+D9+E9)</f>
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -6884,16 +6884,16 @@
       <c r="G10" s="2"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="91" t="s">
+      <c r="C15" s="104" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="92"/>
-      <c r="E15" s="93"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="106"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="94"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="96"/>
+      <c r="C16" s="107"/>
+      <c r="D16" s="108"/>
+      <c r="E16" s="109"/>
       <c r="G16" t="s">
         <v>70</v>
       </c>
@@ -6903,15 +6903,15 @@
     </row>
     <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="97" t="s">
+      <c r="B18" s="110" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="98"/>
-      <c r="D18" s="99"/>
-      <c r="E18" s="100" t="s">
+      <c r="C18" s="111"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="113" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="101"/>
+      <c r="F18" s="114"/>
       <c r="G18" s="42" t="s">
         <v>1</v>
       </c>
@@ -6926,15 +6926,15 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="79" t="s">
+      <c r="B19" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="80"/>
-      <c r="D19" s="108"/>
-      <c r="E19" s="89" t="s">
+      <c r="C19" s="67"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="101" t="s">
         <v>77</v>
       </c>
-      <c r="F19" s="90"/>
+      <c r="F19" s="102"/>
       <c r="G19" s="34"/>
       <c r="H19" s="34">
         <v>0</v>
@@ -6945,13 +6945,13 @@
       <c r="J19" s="35"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="71"/>
-      <c r="C20" s="72"/>
-      <c r="D20" s="109"/>
-      <c r="E20" s="89" t="s">
+      <c r="B20" s="69"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="101" t="s">
         <v>78</v>
       </c>
-      <c r="F20" s="90"/>
+      <c r="F20" s="102"/>
       <c r="G20" s="34">
         <v>4</v>
       </c>
@@ -6961,16 +6961,18 @@
       <c r="I20" s="34">
         <v>2</v>
       </c>
-      <c r="J20" s="35"/>
+      <c r="J20" s="35">
+        <v>6</v>
+      </c>
     </row>
     <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="71"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="109"/>
-      <c r="E21" s="89" t="s">
+      <c r="B21" s="69"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="96"/>
+      <c r="E21" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="F21" s="90"/>
+      <c r="F21" s="102"/>
       <c r="G21" s="34">
         <v>8</v>
       </c>
@@ -6983,13 +6985,13 @@
       <c r="J21" s="35"/>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="71"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="109"/>
-      <c r="E22" s="89" t="s">
+      <c r="B22" s="69"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="101" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="90"/>
+      <c r="F22" s="102"/>
       <c r="G22" s="34"/>
       <c r="H22" s="34">
         <v>0</v>
@@ -7000,13 +7002,13 @@
       <c r="J22" s="35"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="82"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="110"/>
-      <c r="E23" s="89" t="s">
+      <c r="B23" s="72"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="97"/>
+      <c r="E23" s="101" t="s">
         <v>81</v>
       </c>
-      <c r="F23" s="90"/>
+      <c r="F23" s="102"/>
       <c r="G23" s="34"/>
       <c r="H23" s="34">
         <v>0</v>
@@ -7017,11 +7019,11 @@
       <c r="J23" s="35"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="79" t="s">
+      <c r="B24" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="80"/>
-      <c r="D24" s="108"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="95"/>
       <c r="E24" s="45" t="s">
         <v>82</v>
       </c>
@@ -7038,9 +7040,9 @@
       <c r="J24" s="35"/>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="82"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="110"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="97"/>
       <c r="E25" s="45" t="s">
         <v>76</v>
       </c>
@@ -7057,79 +7059,79 @@
       <c r="J25" s="35"/>
     </row>
     <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="111"/>
-      <c r="C26" s="112"/>
-      <c r="D26" s="113"/>
-      <c r="E26" s="89"/>
-      <c r="F26" s="90"/>
+      <c r="B26" s="98"/>
+      <c r="C26" s="99"/>
+      <c r="D26" s="100"/>
+      <c r="E26" s="101"/>
+      <c r="F26" s="102"/>
       <c r="G26" s="34"/>
       <c r="H26" s="34"/>
       <c r="I26" s="34"/>
       <c r="J26" s="35"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="111"/>
-      <c r="C27" s="112"/>
-      <c r="D27" s="113"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="90"/>
+      <c r="B27" s="98"/>
+      <c r="C27" s="99"/>
+      <c r="D27" s="100"/>
+      <c r="E27" s="101"/>
+      <c r="F27" s="102"/>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
       <c r="J27" s="35"/>
     </row>
     <row r="28" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="111"/>
-      <c r="C28" s="112"/>
-      <c r="D28" s="113"/>
-      <c r="E28" s="89"/>
-      <c r="F28" s="90"/>
+      <c r="B28" s="98"/>
+      <c r="C28" s="99"/>
+      <c r="D28" s="100"/>
+      <c r="E28" s="101"/>
+      <c r="F28" s="102"/>
       <c r="G28" s="34"/>
       <c r="H28" s="34"/>
       <c r="I28" s="34"/>
       <c r="J28" s="35"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="111"/>
-      <c r="C29" s="112"/>
-      <c r="D29" s="113"/>
-      <c r="E29" s="89"/>
-      <c r="F29" s="90"/>
+      <c r="B29" s="98"/>
+      <c r="C29" s="99"/>
+      <c r="D29" s="100"/>
+      <c r="E29" s="101"/>
+      <c r="F29" s="102"/>
       <c r="G29" s="34"/>
       <c r="H29" s="34"/>
       <c r="I29" s="34"/>
       <c r="J29" s="35"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="85"/>
-      <c r="C30" s="86"/>
-      <c r="D30" s="114"/>
-      <c r="E30" s="89"/>
-      <c r="F30" s="90"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="76"/>
+      <c r="D30" s="103"/>
+      <c r="E30" s="101"/>
+      <c r="F30" s="102"/>
       <c r="G30" s="34"/>
       <c r="H30" s="34"/>
       <c r="I30" s="34"/>
       <c r="J30" s="35"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="85"/>
-      <c r="C31" s="86"/>
-      <c r="D31" s="114"/>
-      <c r="E31" s="89"/>
-      <c r="F31" s="90"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="103"/>
+      <c r="E31" s="101"/>
+      <c r="F31" s="102"/>
       <c r="G31" s="34"/>
       <c r="H31" s="34"/>
       <c r="I31" s="34"/>
       <c r="J31" s="35"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="102" t="s">
+      <c r="B32" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="103"/>
-      <c r="D32" s="103"/>
-      <c r="E32" s="103"/>
-      <c r="F32" s="104"/>
+      <c r="C32" s="90"/>
+      <c r="D32" s="90"/>
+      <c r="E32" s="90"/>
+      <c r="F32" s="91"/>
       <c r="G32" s="38">
         <f>SUM(G19:G31)</f>
         <v>17</v>
@@ -7148,13 +7150,13 @@
       </c>
     </row>
     <row r="33" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="105" t="s">
+      <c r="B33" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="106"/>
-      <c r="D33" s="106"/>
-      <c r="E33" s="106"/>
-      <c r="F33" s="107"/>
+      <c r="C33" s="93"/>
+      <c r="D33" s="93"/>
+      <c r="E33" s="93"/>
+      <c r="F33" s="94"/>
       <c r="G33" s="40">
         <f>SUM(G19:G31)</f>
         <v>17</v>
@@ -7169,11 +7171,20 @@
       </c>
       <c r="J33" s="41">
         <f>G33-SUM(H19:J31)</f>
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C15:E16"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
     <mergeCell ref="B32:F32"/>
     <mergeCell ref="B33:F33"/>
     <mergeCell ref="B19:D23"/>
@@ -7190,15 +7201,6 @@
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C15:E16"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -7226,11 +7228,11 @@
     <row r="1" spans="2:8" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="59"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="54"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
@@ -7335,16 +7337,16 @@
       <c r="G10" s="2"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="91" t="s">
+      <c r="C15" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="92"/>
-      <c r="E15" s="93"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="106"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="94"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="96"/>
+      <c r="C16" s="107"/>
+      <c r="D16" s="108"/>
+      <c r="E16" s="109"/>
       <c r="G16" t="s">
         <v>70</v>
       </c>
@@ -7354,15 +7356,15 @@
     </row>
     <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="97" t="s">
+      <c r="B18" s="110" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="98"/>
-      <c r="D18" s="99"/>
-      <c r="E18" s="100" t="s">
+      <c r="C18" s="111"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="113" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="101"/>
+      <c r="F18" s="114"/>
       <c r="G18" s="42" t="s">
         <v>1</v>
       </c>
@@ -7377,24 +7379,24 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="79" t="s">
+      <c r="B19" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="80"/>
-      <c r="D19" s="108"/>
-      <c r="E19" s="89" t="s">
+      <c r="C19" s="67"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="101" t="s">
         <v>84</v>
       </c>
-      <c r="F19" s="90"/>
+      <c r="F19" s="102"/>
       <c r="G19" s="34"/>
       <c r="H19" s="34"/>
       <c r="I19" s="34"/>
       <c r="J19" s="35"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="71"/>
-      <c r="C20" s="72"/>
-      <c r="D20" s="109"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="96"/>
       <c r="E20" s="45" t="s">
         <v>87</v>
       </c>
@@ -7405,9 +7407,9 @@
       <c r="J20" s="35"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="71"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="109"/>
+      <c r="B21" s="69"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="96"/>
       <c r="E21" s="45" t="s">
         <v>88</v>
       </c>
@@ -7418,9 +7420,9 @@
       <c r="J21" s="35"/>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="71"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="109"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="96"/>
       <c r="E22" s="45" t="s">
         <v>89</v>
       </c>
@@ -7431,9 +7433,9 @@
       <c r="J22" s="35"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="71"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="109"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="96"/>
       <c r="E23" s="45" t="s">
         <v>90</v>
       </c>
@@ -7444,9 +7446,9 @@
       <c r="J23" s="35"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="71"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="109"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="96"/>
       <c r="E24" s="45" t="s">
         <v>91</v>
       </c>
@@ -7457,9 +7459,9 @@
       <c r="J24" s="35"/>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="82"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="110"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="97"/>
       <c r="E25" s="45" t="s">
         <v>92</v>
       </c>
@@ -7470,122 +7472,122 @@
       <c r="J25" s="35"/>
     </row>
     <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="111" t="s">
+      <c r="B26" s="98" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="112"/>
-      <c r="D26" s="113"/>
-      <c r="E26" s="89" t="s">
+      <c r="C26" s="99"/>
+      <c r="D26" s="100"/>
+      <c r="E26" s="101" t="s">
         <v>83</v>
       </c>
-      <c r="F26" s="90"/>
+      <c r="F26" s="102"/>
       <c r="G26" s="34"/>
       <c r="H26" s="34"/>
       <c r="I26" s="34"/>
       <c r="J26" s="35"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="79" t="s">
+      <c r="B27" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="80"/>
-      <c r="D27" s="108"/>
-      <c r="E27" s="89" t="s">
+      <c r="C27" s="67"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="101" t="s">
         <v>85</v>
       </c>
-      <c r="F27" s="90"/>
+      <c r="F27" s="102"/>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
       <c r="J27" s="35"/>
     </row>
     <row r="28" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="82"/>
-      <c r="C28" s="83"/>
-      <c r="D28" s="110"/>
-      <c r="E28" s="89" t="s">
+      <c r="B28" s="72"/>
+      <c r="C28" s="73"/>
+      <c r="D28" s="97"/>
+      <c r="E28" s="101" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="90"/>
+      <c r="F28" s="102"/>
       <c r="G28" s="34"/>
       <c r="H28" s="34"/>
       <c r="I28" s="34"/>
       <c r="J28" s="35"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="111"/>
-      <c r="C29" s="112"/>
-      <c r="D29" s="113"/>
-      <c r="E29" s="89"/>
-      <c r="F29" s="90"/>
+      <c r="B29" s="98"/>
+      <c r="C29" s="99"/>
+      <c r="D29" s="100"/>
+      <c r="E29" s="101"/>
+      <c r="F29" s="102"/>
       <c r="G29" s="34"/>
       <c r="H29" s="34"/>
       <c r="I29" s="34"/>
       <c r="J29" s="35"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="111"/>
-      <c r="C30" s="112"/>
-      <c r="D30" s="113"/>
-      <c r="E30" s="89"/>
-      <c r="F30" s="90"/>
+      <c r="B30" s="98"/>
+      <c r="C30" s="99"/>
+      <c r="D30" s="100"/>
+      <c r="E30" s="101"/>
+      <c r="F30" s="102"/>
       <c r="G30" s="34"/>
       <c r="H30" s="34"/>
       <c r="I30" s="34"/>
       <c r="J30" s="35"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="111"/>
-      <c r="C31" s="112"/>
-      <c r="D31" s="113"/>
-      <c r="E31" s="89"/>
-      <c r="F31" s="90"/>
+      <c r="B31" s="98"/>
+      <c r="C31" s="99"/>
+      <c r="D31" s="100"/>
+      <c r="E31" s="101"/>
+      <c r="F31" s="102"/>
       <c r="G31" s="34"/>
       <c r="H31" s="34"/>
       <c r="I31" s="34"/>
       <c r="J31" s="35"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="111"/>
-      <c r="C32" s="112"/>
-      <c r="D32" s="113"/>
-      <c r="E32" s="89"/>
-      <c r="F32" s="90"/>
+      <c r="B32" s="98"/>
+      <c r="C32" s="99"/>
+      <c r="D32" s="100"/>
+      <c r="E32" s="101"/>
+      <c r="F32" s="102"/>
       <c r="G32" s="34"/>
       <c r="H32" s="34"/>
       <c r="I32" s="34"/>
       <c r="J32" s="35"/>
     </row>
     <row r="33" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="85"/>
-      <c r="C33" s="86"/>
-      <c r="D33" s="114"/>
-      <c r="E33" s="89"/>
-      <c r="F33" s="90"/>
+      <c r="B33" s="75"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="103"/>
+      <c r="E33" s="101"/>
+      <c r="F33" s="102"/>
       <c r="G33" s="34"/>
       <c r="H33" s="34"/>
       <c r="I33" s="34"/>
       <c r="J33" s="35"/>
     </row>
     <row r="34" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="85"/>
-      <c r="C34" s="86"/>
-      <c r="D34" s="114"/>
-      <c r="E34" s="89"/>
-      <c r="F34" s="90"/>
+      <c r="B34" s="75"/>
+      <c r="C34" s="76"/>
+      <c r="D34" s="103"/>
+      <c r="E34" s="101"/>
+      <c r="F34" s="102"/>
       <c r="G34" s="34"/>
       <c r="H34" s="34"/>
       <c r="I34" s="34"/>
       <c r="J34" s="35"/>
     </row>
     <row r="35" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="102" t="s">
+      <c r="B35" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="103"/>
-      <c r="D35" s="103"/>
-      <c r="E35" s="103"/>
-      <c r="F35" s="104"/>
+      <c r="C35" s="90"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="90"/>
+      <c r="F35" s="91"/>
       <c r="G35" s="38">
         <f>SUM(G19:G34)</f>
         <v>0</v>
@@ -7604,13 +7606,13 @@
       </c>
     </row>
     <row r="36" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="105" t="s">
+      <c r="B36" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="106"/>
-      <c r="D36" s="106"/>
-      <c r="E36" s="106"/>
-      <c r="F36" s="107"/>
+      <c r="C36" s="93"/>
+      <c r="D36" s="93"/>
+      <c r="E36" s="93"/>
+      <c r="F36" s="94"/>
       <c r="G36" s="40">
         <f>SUM(G19:G34)</f>
         <v>0</v>
@@ -7630,6 +7632,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C15:E16"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
     <mergeCell ref="B35:F35"/>
     <mergeCell ref="B36:F36"/>
     <mergeCell ref="B27:D28"/>
@@ -7646,15 +7657,6 @@
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="E31:F31"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C15:E16"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Update files for submission
</commit_message>
<xml_diff>
--- a/ProjectPlanning_Current.xlsx
+++ b/ProjectPlanning_Current.xlsx
@@ -5,7 +5,7 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kamakazi\Documents\MAD\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim\AndroidStudioProjects\MAD\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -1221,6 +1221,26 @@
     <xf numFmtId="0" fontId="10" fillId="14" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1230,78 +1250,7 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1322,7 +1271,89 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1359,40 +1390,9 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -2471,7 +2471,7 @@
                   <c:v>29</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5213,7 +5213,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T31"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
@@ -5225,11 +5225,11 @@
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="52" t="s">
+      <c r="C1" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="53"/>
-      <c r="E1" s="54"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="59"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="1"/>
@@ -5476,14 +5476,14 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="59" t="s">
+      <c r="D11" s="54" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="59"/>
-      <c r="F11" s="59"/>
-      <c r="G11" s="59"/>
-      <c r="H11" s="59"/>
-      <c r="I11" s="59"/>
+      <c r="E11" s="54"/>
+      <c r="F11" s="54"/>
+      <c r="G11" s="54"/>
+      <c r="H11" s="54"/>
+      <c r="I11" s="54"/>
       <c r="J11" s="1"/>
       <c r="K11" s="20" t="s">
         <v>33</v>
@@ -5518,10 +5518,10 @@
     </row>
     <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="60" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="56"/>
+      <c r="C13" s="61"/>
       <c r="D13" s="17" t="s">
         <v>0</v>
       </c>
@@ -5548,10 +5548,10 @@
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="58"/>
+      <c r="C14" s="53"/>
       <c r="D14" s="18" t="s">
         <v>6</v>
       </c>
@@ -5578,10 +5578,10 @@
     </row>
     <row r="15" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="58"/>
+      <c r="C15" s="53"/>
       <c r="D15" s="18" t="s">
         <v>7</v>
       </c>
@@ -5608,10 +5608,10 @@
     </row>
     <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="58"/>
+      <c r="C16" s="53"/>
       <c r="D16" s="18" t="s">
         <v>8</v>
       </c>
@@ -5638,10 +5638,10 @@
     </row>
     <row r="17" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="58"/>
+      <c r="C17" s="53"/>
       <c r="D17" s="18" t="s">
         <v>9</v>
       </c>
@@ -5668,10 +5668,10 @@
     </row>
     <row r="18" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="52" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="58"/>
+      <c r="C18" s="53"/>
       <c r="D18" s="18" t="s">
         <v>10</v>
       </c>
@@ -5698,10 +5698,10 @@
     </row>
     <row r="19" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="57" t="s">
+      <c r="B19" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="58"/>
+      <c r="C19" s="53"/>
       <c r="D19" s="18" t="s">
         <v>11</v>
       </c>
@@ -5728,10 +5728,10 @@
     </row>
     <row r="20" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="57" t="s">
+      <c r="B20" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="58"/>
+      <c r="C20" s="53"/>
       <c r="D20" s="18" t="s">
         <v>12</v>
       </c>
@@ -5758,10 +5758,10 @@
     </row>
     <row r="21" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="57" t="s">
+      <c r="B21" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="58"/>
+      <c r="C21" s="53"/>
       <c r="D21" s="18" t="s">
         <v>13</v>
       </c>
@@ -5788,10 +5788,10 @@
     </row>
     <row r="22" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="57" t="s">
+      <c r="B22" s="52" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="58"/>
+      <c r="C22" s="53"/>
       <c r="D22" s="18" t="s">
         <v>14</v>
       </c>
@@ -5818,10 +5818,10 @@
     </row>
     <row r="23" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="B23" s="57" t="s">
+      <c r="B23" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="58"/>
+      <c r="C23" s="53"/>
       <c r="D23" s="18" t="s">
         <v>15</v>
       </c>
@@ -5848,10 +5848,10 @@
     </row>
     <row r="24" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="57" t="s">
+      <c r="B24" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="58"/>
+      <c r="C24" s="53"/>
       <c r="D24" s="18" t="s">
         <v>16</v>
       </c>
@@ -5878,10 +5878,10 @@
     </row>
     <row r="25" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="57" t="s">
+      <c r="B25" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="58"/>
+      <c r="C25" s="53"/>
       <c r="D25" s="18" t="s">
         <v>17</v>
       </c>
@@ -5908,10 +5908,10 @@
     </row>
     <row r="26" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="57" t="s">
+      <c r="B26" s="52" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="58"/>
+      <c r="C26" s="53"/>
       <c r="D26" s="18" t="s">
         <v>18</v>
       </c>
@@ -5938,11 +5938,11 @@
     </row>
     <row r="27" spans="1:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="60" t="s">
+      <c r="B27" s="55" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="61"/>
-      <c r="D27" s="61"/>
+      <c r="C27" s="56"/>
+      <c r="D27" s="56"/>
       <c r="E27" s="19">
         <f>SUM(E14:E26)</f>
         <v>40</v>
@@ -5972,11 +5972,11 @@
     </row>
     <row r="28" spans="1:20" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="60" t="s">
+      <c r="B28" s="55" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="61"/>
-      <c r="D28" s="61"/>
+      <c r="C28" s="56"/>
+      <c r="D28" s="56"/>
       <c r="E28" s="19">
         <f>SUM(E14:E26)</f>
         <v>40</v>
@@ -6067,6 +6067,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="D11:I11"/>
@@ -6080,11 +6085,6 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6098,7 +6098,7 @@
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6281,7 +6281,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:K31"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
@@ -6297,11 +6297,11 @@
     <row r="1" spans="2:9" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="54"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="59"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
@@ -6430,18 +6430,18 @@
       <c r="G10" s="2"/>
     </row>
     <row r="15" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="64" t="s">
+      <c r="D15" s="77" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="65"/>
-      <c r="F15" s="65"/>
-      <c r="G15" s="65"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="78"/>
     </row>
     <row r="16" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="64"/>
-      <c r="E16" s="65"/>
-      <c r="F16" s="65"/>
-      <c r="G16" s="65"/>
+      <c r="D16" s="77"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
       <c r="H16" t="s">
         <v>70</v>
       </c>
@@ -6451,15 +6451,15 @@
     </row>
     <row r="17" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="3:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="80" t="s">
+      <c r="C18" s="63" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="81"/>
-      <c r="E18" s="82"/>
-      <c r="F18" s="83" t="s">
+      <c r="D18" s="64"/>
+      <c r="E18" s="65"/>
+      <c r="F18" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="84"/>
+      <c r="G18" s="67"/>
       <c r="H18" s="48" t="s">
         <v>1</v>
       </c>
@@ -6474,15 +6474,15 @@
       </c>
     </row>
     <row r="19" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C19" s="85" t="s">
+      <c r="C19" s="68" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="86"/>
-      <c r="E19" s="87"/>
-      <c r="F19" s="88" t="s">
+      <c r="D19" s="69"/>
+      <c r="E19" s="70"/>
+      <c r="F19" s="74" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="88"/>
+      <c r="G19" s="74"/>
       <c r="H19" s="50">
         <v>2</v>
       </c>
@@ -6497,13 +6497,13 @@
       </c>
     </row>
     <row r="20" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C20" s="69"/>
-      <c r="D20" s="70"/>
-      <c r="E20" s="71"/>
-      <c r="F20" s="77" t="s">
+      <c r="C20" s="71"/>
+      <c r="D20" s="72"/>
+      <c r="E20" s="73"/>
+      <c r="F20" s="62" t="s">
         <v>67</v>
       </c>
-      <c r="G20" s="77"/>
+      <c r="G20" s="62"/>
       <c r="H20" s="36">
         <v>4</v>
       </c>
@@ -6518,15 +6518,15 @@
       </c>
     </row>
     <row r="21" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C21" s="75" t="s">
+      <c r="C21" s="85" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="76"/>
-      <c r="E21" s="76"/>
-      <c r="F21" s="77" t="s">
+      <c r="D21" s="86"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="G21" s="77"/>
+      <c r="G21" s="62"/>
       <c r="H21" s="36">
         <v>1</v>
       </c>
@@ -6541,13 +6541,13 @@
       </c>
     </row>
     <row r="22" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C22" s="75"/>
-      <c r="D22" s="76"/>
-      <c r="E22" s="76"/>
-      <c r="F22" s="77" t="s">
+      <c r="C22" s="85"/>
+      <c r="D22" s="86"/>
+      <c r="E22" s="86"/>
+      <c r="F22" s="62" t="s">
         <v>68</v>
       </c>
-      <c r="G22" s="77"/>
+      <c r="G22" s="62"/>
       <c r="H22" s="36">
         <v>2</v>
       </c>
@@ -6562,9 +6562,9 @@
       </c>
     </row>
     <row r="23" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C23" s="75"/>
-      <c r="D23" s="76"/>
-      <c r="E23" s="76"/>
+      <c r="C23" s="85"/>
+      <c r="D23" s="86"/>
+      <c r="E23" s="86"/>
       <c r="F23" s="47" t="s">
         <v>75</v>
       </c>
@@ -6583,81 +6583,81 @@
       </c>
     </row>
     <row r="24" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C24" s="66" t="s">
+      <c r="C24" s="79" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="67"/>
-      <c r="E24" s="68"/>
-      <c r="F24" s="77"/>
-      <c r="G24" s="77"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="81"/>
+      <c r="F24" s="62"/>
+      <c r="G24" s="62"/>
       <c r="H24" s="36"/>
       <c r="I24" s="36"/>
       <c r="J24" s="36"/>
       <c r="K24" s="37"/>
     </row>
     <row r="25" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C25" s="69"/>
-      <c r="D25" s="70"/>
-      <c r="E25" s="71"/>
-      <c r="F25" s="77"/>
-      <c r="G25" s="77"/>
+      <c r="C25" s="71"/>
+      <c r="D25" s="72"/>
+      <c r="E25" s="73"/>
+      <c r="F25" s="62"/>
+      <c r="G25" s="62"/>
       <c r="H25" s="36"/>
       <c r="I25" s="36"/>
       <c r="J25" s="36"/>
       <c r="K25" s="37"/>
     </row>
     <row r="26" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C26" s="72"/>
-      <c r="D26" s="73"/>
-      <c r="E26" s="74"/>
-      <c r="F26" s="77"/>
-      <c r="G26" s="77"/>
+      <c r="C26" s="82"/>
+      <c r="D26" s="83"/>
+      <c r="E26" s="84"/>
+      <c r="F26" s="62"/>
+      <c r="G26" s="62"/>
       <c r="H26" s="36"/>
       <c r="I26" s="36"/>
       <c r="J26" s="36"/>
       <c r="K26" s="37"/>
     </row>
     <row r="27" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C27" s="75"/>
-      <c r="D27" s="76"/>
-      <c r="E27" s="76"/>
-      <c r="F27" s="77"/>
-      <c r="G27" s="77"/>
+      <c r="C27" s="85"/>
+      <c r="D27" s="86"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="62"/>
+      <c r="G27" s="62"/>
       <c r="H27" s="36"/>
       <c r="I27" s="36"/>
       <c r="J27" s="36"/>
       <c r="K27" s="37"/>
     </row>
     <row r="28" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C28" s="75"/>
-      <c r="D28" s="76"/>
-      <c r="E28" s="76"/>
-      <c r="F28" s="77"/>
-      <c r="G28" s="77"/>
+      <c r="C28" s="85"/>
+      <c r="D28" s="86"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="62"/>
+      <c r="G28" s="62"/>
       <c r="H28" s="36"/>
       <c r="I28" s="36"/>
       <c r="J28" s="36"/>
       <c r="K28" s="37"/>
     </row>
     <row r="29" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C29" s="75"/>
-      <c r="D29" s="76"/>
-      <c r="E29" s="76"/>
-      <c r="F29" s="77"/>
-      <c r="G29" s="77"/>
+      <c r="C29" s="85"/>
+      <c r="D29" s="86"/>
+      <c r="E29" s="86"/>
+      <c r="F29" s="62"/>
+      <c r="G29" s="62"/>
       <c r="H29" s="36"/>
       <c r="I29" s="36"/>
       <c r="J29" s="36"/>
       <c r="K29" s="37"/>
     </row>
     <row r="30" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C30" s="78" t="s">
+      <c r="C30" s="87" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="79"/>
-      <c r="E30" s="79"/>
-      <c r="F30" s="79"/>
-      <c r="G30" s="79"/>
+      <c r="D30" s="88"/>
+      <c r="E30" s="88"/>
+      <c r="F30" s="88"/>
+      <c r="G30" s="88"/>
       <c r="H30" s="38">
         <f>SUM(H19:H29)</f>
         <v>11</v>
@@ -6676,13 +6676,13 @@
       </c>
     </row>
     <row r="31" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="62" t="s">
+      <c r="C31" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="D31" s="63"/>
-      <c r="E31" s="63"/>
-      <c r="F31" s="63"/>
-      <c r="G31" s="63"/>
+      <c r="D31" s="76"/>
+      <c r="E31" s="76"/>
+      <c r="F31" s="76"/>
+      <c r="G31" s="76"/>
       <c r="H31" s="40">
         <f>SUM(H19:H29)</f>
         <v>11</v>
@@ -6702,14 +6702,6 @@
     </row>
   </sheetData>
   <mergeCells count="22">
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="C19:E20"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
     <mergeCell ref="C31:G31"/>
     <mergeCell ref="D15:G16"/>
     <mergeCell ref="C24:E26"/>
@@ -6724,6 +6716,14 @@
     <mergeCell ref="F27:G27"/>
     <mergeCell ref="C21:E23"/>
     <mergeCell ref="F21:G21"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="C19:E20"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -6735,8 +6735,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6751,11 +6751,11 @@
     <row r="1" spans="2:8" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="54"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="59"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
@@ -6843,11 +6843,11 @@
         <v>6</v>
       </c>
       <c r="E8" s="7">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F8" s="11">
         <f>SUM(C8:E8)</f>
-        <v>12</v>
+        <v>18</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -6865,7 +6865,7 @@
       </c>
       <c r="E9" s="14">
         <f>SUM(E5:E8)</f>
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -6876,7 +6876,7 @@
       </c>
       <c r="C10" s="16">
         <f>SUM(C9+D9+E9)</f>
-        <v>74</v>
+        <v>80</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -6884,16 +6884,16 @@
       <c r="G10" s="2"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="104" t="s">
+      <c r="C15" s="91" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="105"/>
-      <c r="E15" s="106"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="93"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="107"/>
-      <c r="D16" s="108"/>
-      <c r="E16" s="109"/>
+      <c r="C16" s="94"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="96"/>
       <c r="G16" t="s">
         <v>70</v>
       </c>
@@ -6903,15 +6903,15 @@
     </row>
     <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="110" t="s">
+      <c r="B18" s="97" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="111"/>
-      <c r="D18" s="112"/>
-      <c r="E18" s="113" t="s">
+      <c r="C18" s="98"/>
+      <c r="D18" s="99"/>
+      <c r="E18" s="100" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="114"/>
+      <c r="F18" s="101"/>
       <c r="G18" s="42" t="s">
         <v>1</v>
       </c>
@@ -6926,15 +6926,15 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="66" t="s">
+      <c r="B19" s="79" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="67"/>
-      <c r="D19" s="95"/>
-      <c r="E19" s="101" t="s">
+      <c r="C19" s="80"/>
+      <c r="D19" s="108"/>
+      <c r="E19" s="89" t="s">
         <v>77</v>
       </c>
-      <c r="F19" s="102"/>
+      <c r="F19" s="90"/>
       <c r="G19" s="34"/>
       <c r="H19" s="34">
         <v>0</v>
@@ -6945,13 +6945,13 @@
       <c r="J19" s="35"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="69"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="96"/>
-      <c r="E20" s="101" t="s">
+      <c r="B20" s="71"/>
+      <c r="C20" s="72"/>
+      <c r="D20" s="109"/>
+      <c r="E20" s="89" t="s">
         <v>78</v>
       </c>
-      <c r="F20" s="102"/>
+      <c r="F20" s="90"/>
       <c r="G20" s="34">
         <v>4</v>
       </c>
@@ -6961,16 +6961,18 @@
       <c r="I20" s="34">
         <v>2</v>
       </c>
-      <c r="J20" s="35"/>
+      <c r="J20" s="35">
+        <v>4</v>
+      </c>
     </row>
     <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="69"/>
-      <c r="C21" s="70"/>
-      <c r="D21" s="96"/>
-      <c r="E21" s="101" t="s">
+      <c r="B21" s="71"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="109"/>
+      <c r="E21" s="89" t="s">
         <v>79</v>
       </c>
-      <c r="F21" s="102"/>
+      <c r="F21" s="90"/>
       <c r="G21" s="34">
         <v>8</v>
       </c>
@@ -6985,13 +6987,13 @@
       </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="69"/>
-      <c r="C22" s="70"/>
-      <c r="D22" s="96"/>
-      <c r="E22" s="101" t="s">
+      <c r="B22" s="71"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="109"/>
+      <c r="E22" s="89" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="102"/>
+      <c r="F22" s="90"/>
       <c r="G22" s="34">
         <v>20</v>
       </c>
@@ -7006,13 +7008,13 @@
       </c>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="72"/>
-      <c r="C23" s="73"/>
-      <c r="D23" s="97"/>
-      <c r="E23" s="101" t="s">
+      <c r="B23" s="82"/>
+      <c r="C23" s="83"/>
+      <c r="D23" s="110"/>
+      <c r="E23" s="89" t="s">
         <v>81</v>
       </c>
-      <c r="F23" s="102"/>
+      <c r="F23" s="90"/>
       <c r="G23" s="34"/>
       <c r="H23" s="34">
         <v>0</v>
@@ -7023,11 +7025,11 @@
       <c r="J23" s="35"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="66" t="s">
+      <c r="B24" s="79" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="67"/>
-      <c r="D24" s="95"/>
+      <c r="C24" s="80"/>
+      <c r="D24" s="108"/>
       <c r="E24" s="45" t="s">
         <v>82</v>
       </c>
@@ -7046,9 +7048,9 @@
       </c>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="72"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="97"/>
+      <c r="B25" s="82"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="110"/>
       <c r="E25" s="45" t="s">
         <v>76</v>
       </c>
@@ -7067,79 +7069,79 @@
       </c>
     </row>
     <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="98"/>
-      <c r="C26" s="99"/>
-      <c r="D26" s="100"/>
-      <c r="E26" s="101"/>
-      <c r="F26" s="102"/>
+      <c r="B26" s="111"/>
+      <c r="C26" s="112"/>
+      <c r="D26" s="113"/>
+      <c r="E26" s="89"/>
+      <c r="F26" s="90"/>
       <c r="G26" s="34"/>
       <c r="H26" s="34"/>
       <c r="I26" s="34"/>
       <c r="J26" s="35"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="98"/>
-      <c r="C27" s="99"/>
-      <c r="D27" s="100"/>
-      <c r="E27" s="101"/>
-      <c r="F27" s="102"/>
+      <c r="B27" s="111"/>
+      <c r="C27" s="112"/>
+      <c r="D27" s="113"/>
+      <c r="E27" s="89"/>
+      <c r="F27" s="90"/>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
       <c r="J27" s="35"/>
     </row>
     <row r="28" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="98"/>
-      <c r="C28" s="99"/>
-      <c r="D28" s="100"/>
-      <c r="E28" s="101"/>
-      <c r="F28" s="102"/>
+      <c r="B28" s="111"/>
+      <c r="C28" s="112"/>
+      <c r="D28" s="113"/>
+      <c r="E28" s="89"/>
+      <c r="F28" s="90"/>
       <c r="G28" s="34"/>
       <c r="H28" s="34"/>
       <c r="I28" s="34"/>
       <c r="J28" s="35"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="98"/>
-      <c r="C29" s="99"/>
-      <c r="D29" s="100"/>
-      <c r="E29" s="101"/>
-      <c r="F29" s="102"/>
+      <c r="B29" s="111"/>
+      <c r="C29" s="112"/>
+      <c r="D29" s="113"/>
+      <c r="E29" s="89"/>
+      <c r="F29" s="90"/>
       <c r="G29" s="34"/>
       <c r="H29" s="34"/>
       <c r="I29" s="34"/>
       <c r="J29" s="35"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="75"/>
-      <c r="C30" s="76"/>
-      <c r="D30" s="103"/>
-      <c r="E30" s="101"/>
-      <c r="F30" s="102"/>
+      <c r="B30" s="85"/>
+      <c r="C30" s="86"/>
+      <c r="D30" s="114"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="90"/>
       <c r="G30" s="34"/>
       <c r="H30" s="34"/>
       <c r="I30" s="34"/>
       <c r="J30" s="35"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="75"/>
-      <c r="C31" s="76"/>
-      <c r="D31" s="103"/>
-      <c r="E31" s="101"/>
-      <c r="F31" s="102"/>
+      <c r="B31" s="85"/>
+      <c r="C31" s="86"/>
+      <c r="D31" s="114"/>
+      <c r="E31" s="89"/>
+      <c r="F31" s="90"/>
       <c r="G31" s="34"/>
       <c r="H31" s="34"/>
       <c r="I31" s="34"/>
       <c r="J31" s="35"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="89" t="s">
+      <c r="B32" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="90"/>
-      <c r="D32" s="90"/>
-      <c r="E32" s="90"/>
-      <c r="F32" s="91"/>
+      <c r="C32" s="103"/>
+      <c r="D32" s="103"/>
+      <c r="E32" s="103"/>
+      <c r="F32" s="104"/>
       <c r="G32" s="38">
         <f>SUM(G19:G31)</f>
         <v>38</v>
@@ -7158,13 +7160,13 @@
       </c>
     </row>
     <row r="33" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="92" t="s">
+      <c r="B33" s="105" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="93"/>
-      <c r="D33" s="93"/>
-      <c r="E33" s="93"/>
-      <c r="F33" s="94"/>
+      <c r="C33" s="106"/>
+      <c r="D33" s="106"/>
+      <c r="E33" s="106"/>
+      <c r="F33" s="107"/>
       <c r="G33" s="40">
         <f>SUM(G19:G31)</f>
         <v>38</v>
@@ -7179,20 +7181,11 @@
       </c>
       <c r="J33" s="41">
         <f>G33-SUM(H19:J31)</f>
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C15:E16"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
     <mergeCell ref="B32:F32"/>
     <mergeCell ref="B33:F33"/>
     <mergeCell ref="B19:D23"/>
@@ -7209,6 +7202,15 @@
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="E28:F28"/>
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C15:E16"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -7236,11 +7238,11 @@
     <row r="1" spans="2:8" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
-      <c r="C3" s="52" t="s">
+      <c r="C3" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="53"/>
-      <c r="E3" s="54"/>
+      <c r="D3" s="58"/>
+      <c r="E3" s="59"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
@@ -7345,16 +7347,16 @@
       <c r="G10" s="2"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="104" t="s">
+      <c r="C15" s="91" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="105"/>
-      <c r="E15" s="106"/>
+      <c r="D15" s="92"/>
+      <c r="E15" s="93"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="107"/>
-      <c r="D16" s="108"/>
-      <c r="E16" s="109"/>
+      <c r="C16" s="94"/>
+      <c r="D16" s="95"/>
+      <c r="E16" s="96"/>
       <c r="G16" t="s">
         <v>70</v>
       </c>
@@ -7364,15 +7366,15 @@
     </row>
     <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="110" t="s">
+      <c r="B18" s="97" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="111"/>
-      <c r="D18" s="112"/>
-      <c r="E18" s="113" t="s">
+      <c r="C18" s="98"/>
+      <c r="D18" s="99"/>
+      <c r="E18" s="100" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="114"/>
+      <c r="F18" s="101"/>
       <c r="G18" s="42" t="s">
         <v>1</v>
       </c>
@@ -7387,24 +7389,24 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="66" t="s">
+      <c r="B19" s="79" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="67"/>
-      <c r="D19" s="95"/>
-      <c r="E19" s="101" t="s">
+      <c r="C19" s="80"/>
+      <c r="D19" s="108"/>
+      <c r="E19" s="89" t="s">
         <v>84</v>
       </c>
-      <c r="F19" s="102"/>
+      <c r="F19" s="90"/>
       <c r="G19" s="34"/>
       <c r="H19" s="34"/>
       <c r="I19" s="34"/>
       <c r="J19" s="35"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="69"/>
-      <c r="C20" s="70"/>
-      <c r="D20" s="96"/>
+      <c r="B20" s="71"/>
+      <c r="C20" s="72"/>
+      <c r="D20" s="109"/>
       <c r="E20" s="45" t="s">
         <v>87</v>
       </c>
@@ -7415,9 +7417,9 @@
       <c r="J20" s="35"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="69"/>
-      <c r="C21" s="70"/>
-      <c r="D21" s="96"/>
+      <c r="B21" s="71"/>
+      <c r="C21" s="72"/>
+      <c r="D21" s="109"/>
       <c r="E21" s="45" t="s">
         <v>88</v>
       </c>
@@ -7428,9 +7430,9 @@
       <c r="J21" s="35"/>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="69"/>
-      <c r="C22" s="70"/>
-      <c r="D22" s="96"/>
+      <c r="B22" s="71"/>
+      <c r="C22" s="72"/>
+      <c r="D22" s="109"/>
       <c r="E22" s="45" t="s">
         <v>89</v>
       </c>
@@ -7441,9 +7443,9 @@
       <c r="J22" s="35"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="69"/>
-      <c r="C23" s="70"/>
-      <c r="D23" s="96"/>
+      <c r="B23" s="71"/>
+      <c r="C23" s="72"/>
+      <c r="D23" s="109"/>
       <c r="E23" s="45" t="s">
         <v>90</v>
       </c>
@@ -7454,9 +7456,9 @@
       <c r="J23" s="35"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="69"/>
-      <c r="C24" s="70"/>
-      <c r="D24" s="96"/>
+      <c r="B24" s="71"/>
+      <c r="C24" s="72"/>
+      <c r="D24" s="109"/>
       <c r="E24" s="45" t="s">
         <v>91</v>
       </c>
@@ -7467,9 +7469,9 @@
       <c r="J24" s="35"/>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="72"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="97"/>
+      <c r="B25" s="82"/>
+      <c r="C25" s="83"/>
+      <c r="D25" s="110"/>
       <c r="E25" s="45" t="s">
         <v>92</v>
       </c>
@@ -7480,122 +7482,122 @@
       <c r="J25" s="35"/>
     </row>
     <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="98" t="s">
+      <c r="B26" s="111" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="99"/>
-      <c r="D26" s="100"/>
-      <c r="E26" s="101" t="s">
+      <c r="C26" s="112"/>
+      <c r="D26" s="113"/>
+      <c r="E26" s="89" t="s">
         <v>83</v>
       </c>
-      <c r="F26" s="102"/>
+      <c r="F26" s="90"/>
       <c r="G26" s="34"/>
       <c r="H26" s="34"/>
       <c r="I26" s="34"/>
       <c r="J26" s="35"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="66" t="s">
+      <c r="B27" s="79" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="67"/>
-      <c r="D27" s="95"/>
-      <c r="E27" s="101" t="s">
+      <c r="C27" s="80"/>
+      <c r="D27" s="108"/>
+      <c r="E27" s="89" t="s">
         <v>85</v>
       </c>
-      <c r="F27" s="102"/>
+      <c r="F27" s="90"/>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
       <c r="J27" s="35"/>
     </row>
     <row r="28" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="72"/>
-      <c r="C28" s="73"/>
-      <c r="D28" s="97"/>
-      <c r="E28" s="101" t="s">
+      <c r="B28" s="82"/>
+      <c r="C28" s="83"/>
+      <c r="D28" s="110"/>
+      <c r="E28" s="89" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="102"/>
+      <c r="F28" s="90"/>
       <c r="G28" s="34"/>
       <c r="H28" s="34"/>
       <c r="I28" s="34"/>
       <c r="J28" s="35"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="98"/>
-      <c r="C29" s="99"/>
-      <c r="D29" s="100"/>
-      <c r="E29" s="101"/>
-      <c r="F29" s="102"/>
+      <c r="B29" s="111"/>
+      <c r="C29" s="112"/>
+      <c r="D29" s="113"/>
+      <c r="E29" s="89"/>
+      <c r="F29" s="90"/>
       <c r="G29" s="34"/>
       <c r="H29" s="34"/>
       <c r="I29" s="34"/>
       <c r="J29" s="35"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="98"/>
-      <c r="C30" s="99"/>
-      <c r="D30" s="100"/>
-      <c r="E30" s="101"/>
-      <c r="F30" s="102"/>
+      <c r="B30" s="111"/>
+      <c r="C30" s="112"/>
+      <c r="D30" s="113"/>
+      <c r="E30" s="89"/>
+      <c r="F30" s="90"/>
       <c r="G30" s="34"/>
       <c r="H30" s="34"/>
       <c r="I30" s="34"/>
       <c r="J30" s="35"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="98"/>
-      <c r="C31" s="99"/>
-      <c r="D31" s="100"/>
-      <c r="E31" s="101"/>
-      <c r="F31" s="102"/>
+      <c r="B31" s="111"/>
+      <c r="C31" s="112"/>
+      <c r="D31" s="113"/>
+      <c r="E31" s="89"/>
+      <c r="F31" s="90"/>
       <c r="G31" s="34"/>
       <c r="H31" s="34"/>
       <c r="I31" s="34"/>
       <c r="J31" s="35"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="98"/>
-      <c r="C32" s="99"/>
-      <c r="D32" s="100"/>
-      <c r="E32" s="101"/>
-      <c r="F32" s="102"/>
+      <c r="B32" s="111"/>
+      <c r="C32" s="112"/>
+      <c r="D32" s="113"/>
+      <c r="E32" s="89"/>
+      <c r="F32" s="90"/>
       <c r="G32" s="34"/>
       <c r="H32" s="34"/>
       <c r="I32" s="34"/>
       <c r="J32" s="35"/>
     </row>
     <row r="33" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="75"/>
-      <c r="C33" s="76"/>
-      <c r="D33" s="103"/>
-      <c r="E33" s="101"/>
-      <c r="F33" s="102"/>
+      <c r="B33" s="85"/>
+      <c r="C33" s="86"/>
+      <c r="D33" s="114"/>
+      <c r="E33" s="89"/>
+      <c r="F33" s="90"/>
       <c r="G33" s="34"/>
       <c r="H33" s="34"/>
       <c r="I33" s="34"/>
       <c r="J33" s="35"/>
     </row>
     <row r="34" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="75"/>
-      <c r="C34" s="76"/>
-      <c r="D34" s="103"/>
-      <c r="E34" s="101"/>
-      <c r="F34" s="102"/>
+      <c r="B34" s="85"/>
+      <c r="C34" s="86"/>
+      <c r="D34" s="114"/>
+      <c r="E34" s="89"/>
+      <c r="F34" s="90"/>
       <c r="G34" s="34"/>
       <c r="H34" s="34"/>
       <c r="I34" s="34"/>
       <c r="J34" s="35"/>
     </row>
     <row r="35" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="89" t="s">
+      <c r="B35" s="102" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="90"/>
-      <c r="D35" s="90"/>
-      <c r="E35" s="90"/>
-      <c r="F35" s="91"/>
+      <c r="C35" s="103"/>
+      <c r="D35" s="103"/>
+      <c r="E35" s="103"/>
+      <c r="F35" s="104"/>
       <c r="G35" s="38">
         <f>SUM(G19:G34)</f>
         <v>0</v>
@@ -7614,13 +7616,13 @@
       </c>
     </row>
     <row r="36" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="92" t="s">
+      <c r="B36" s="105" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="93"/>
-      <c r="D36" s="93"/>
-      <c r="E36" s="93"/>
-      <c r="F36" s="94"/>
+      <c r="C36" s="106"/>
+      <c r="D36" s="106"/>
+      <c r="E36" s="106"/>
+      <c r="F36" s="107"/>
       <c r="G36" s="40">
         <f>SUM(G19:G34)</f>
         <v>0</v>
@@ -7640,15 +7642,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C15:E16"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
     <mergeCell ref="B35:F35"/>
     <mergeCell ref="B36:F36"/>
     <mergeCell ref="B27:D28"/>
@@ -7665,6 +7658,15 @@
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="E31:F31"/>
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C15:E16"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>

<commit_message>
Added some stuff to sprint 3 burndown
</commit_message>
<xml_diff>
--- a/ProjectPlanning_Current.xlsx
+++ b/ProjectPlanning_Current.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5940" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17970" windowHeight="5940" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="BurndownChartTemplate" sheetId="3" r:id="rId1"/>
@@ -1221,26 +1221,6 @@
     <xf numFmtId="0" fontId="10" fillId="14" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -1250,7 +1230,78 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1271,60 +1322,48 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="11" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1354,45 +1393,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="14" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="13" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="12" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="1" builtinId="9" hidden="1"/>
@@ -2837,13 +2837,13 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>5.3333333333333339</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>2.666666666666667</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0</c:v>
@@ -2915,16 +2915,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5225,11 +5225,11 @@
     <row r="1" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="2"/>
-      <c r="C1" s="57" t="s">
+      <c r="C1" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="D1" s="58"/>
-      <c r="E1" s="59"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="54"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
       <c r="H1" s="1"/>
@@ -5476,14 +5476,14 @@
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
-      <c r="D11" s="54" t="s">
+      <c r="D11" s="59" t="s">
         <v>21</v>
       </c>
-      <c r="E11" s="54"/>
-      <c r="F11" s="54"/>
-      <c r="G11" s="54"/>
-      <c r="H11" s="54"/>
-      <c r="I11" s="54"/>
+      <c r="E11" s="59"/>
+      <c r="F11" s="59"/>
+      <c r="G11" s="59"/>
+      <c r="H11" s="59"/>
+      <c r="I11" s="59"/>
       <c r="J11" s="1"/>
       <c r="K11" s="20" t="s">
         <v>33</v>
@@ -5518,10 +5518,10 @@
     </row>
     <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="2"/>
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="55" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="61"/>
+      <c r="C13" s="56"/>
       <c r="D13" s="17" t="s">
         <v>0</v>
       </c>
@@ -5548,10 +5548,10 @@
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="2"/>
-      <c r="B14" s="52" t="s">
+      <c r="B14" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="C14" s="53"/>
+      <c r="C14" s="58"/>
       <c r="D14" s="18" t="s">
         <v>6</v>
       </c>
@@ -5578,10 +5578,10 @@
     </row>
     <row r="15" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="2"/>
-      <c r="B15" s="52" t="s">
+      <c r="B15" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="C15" s="53"/>
+      <c r="C15" s="58"/>
       <c r="D15" s="18" t="s">
         <v>7</v>
       </c>
@@ -5608,10 +5608,10 @@
     </row>
     <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="52" t="s">
+      <c r="B16" s="57" t="s">
         <v>2</v>
       </c>
-      <c r="C16" s="53"/>
+      <c r="C16" s="58"/>
       <c r="D16" s="18" t="s">
         <v>8</v>
       </c>
@@ -5638,10 +5638,10 @@
     </row>
     <row r="17" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="2"/>
-      <c r="B17" s="52" t="s">
+      <c r="B17" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C17" s="53"/>
+      <c r="C17" s="58"/>
       <c r="D17" s="18" t="s">
         <v>9</v>
       </c>
@@ -5668,10 +5668,10 @@
     </row>
     <row r="18" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="2"/>
-      <c r="B18" s="52" t="s">
+      <c r="B18" s="57" t="s">
         <v>3</v>
       </c>
-      <c r="C18" s="53"/>
+      <c r="C18" s="58"/>
       <c r="D18" s="18" t="s">
         <v>10</v>
       </c>
@@ -5698,10 +5698,10 @@
     </row>
     <row r="19" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A19" s="2"/>
-      <c r="B19" s="52" t="s">
+      <c r="B19" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="53"/>
+      <c r="C19" s="58"/>
       <c r="D19" s="18" t="s">
         <v>11</v>
       </c>
@@ -5728,10 +5728,10 @@
     </row>
     <row r="20" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A20" s="2"/>
-      <c r="B20" s="52" t="s">
+      <c r="B20" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C20" s="53"/>
+      <c r="C20" s="58"/>
       <c r="D20" s="18" t="s">
         <v>12</v>
       </c>
@@ -5758,10 +5758,10 @@
     </row>
     <row r="21" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A21" s="2"/>
-      <c r="B21" s="52" t="s">
+      <c r="B21" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C21" s="53"/>
+      <c r="C21" s="58"/>
       <c r="D21" s="18" t="s">
         <v>13</v>
       </c>
@@ -5788,10 +5788,10 @@
     </row>
     <row r="22" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="2"/>
-      <c r="B22" s="52" t="s">
+      <c r="B22" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="C22" s="53"/>
+      <c r="C22" s="58"/>
       <c r="D22" s="18" t="s">
         <v>14</v>
       </c>
@@ -5818,10 +5818,10 @@
     </row>
     <row r="23" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A23" s="2"/>
-      <c r="B23" s="52" t="s">
+      <c r="B23" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="53"/>
+      <c r="C23" s="58"/>
       <c r="D23" s="18" t="s">
         <v>15</v>
       </c>
@@ -5848,10 +5848,10 @@
     </row>
     <row r="24" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="52" t="s">
+      <c r="B24" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="53"/>
+      <c r="C24" s="58"/>
       <c r="D24" s="18" t="s">
         <v>16</v>
       </c>
@@ -5878,10 +5878,10 @@
     </row>
     <row r="25" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="52" t="s">
+      <c r="B25" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="53"/>
+      <c r="C25" s="58"/>
       <c r="D25" s="18" t="s">
         <v>17</v>
       </c>
@@ -5908,10 +5908,10 @@
     </row>
     <row r="26" spans="1:20" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="52" t="s">
+      <c r="B26" s="57" t="s">
         <v>5</v>
       </c>
-      <c r="C26" s="53"/>
+      <c r="C26" s="58"/>
       <c r="D26" s="18" t="s">
         <v>18</v>
       </c>
@@ -5938,11 +5938,11 @@
     </row>
     <row r="27" spans="1:20" ht="29.1" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2"/>
-      <c r="B27" s="55" t="s">
+      <c r="B27" s="60" t="s">
         <v>19</v>
       </c>
-      <c r="C27" s="56"/>
-      <c r="D27" s="56"/>
+      <c r="C27" s="61"/>
+      <c r="D27" s="61"/>
       <c r="E27" s="19">
         <f>SUM(E14:E26)</f>
         <v>40</v>
@@ -5972,11 +5972,11 @@
     </row>
     <row r="28" spans="1:20" ht="27.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2"/>
-      <c r="B28" s="55" t="s">
+      <c r="B28" s="60" t="s">
         <v>20</v>
       </c>
-      <c r="C28" s="56"/>
-      <c r="D28" s="56"/>
+      <c r="C28" s="61"/>
+      <c r="D28" s="61"/>
       <c r="E28" s="19">
         <f>SUM(E14:E26)</f>
         <v>40</v>
@@ -6067,11 +6067,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="C1:E1"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="D11:I11"/>
@@ -6085,6 +6080,11 @@
     <mergeCell ref="B20:C20"/>
     <mergeCell ref="B21:C21"/>
     <mergeCell ref="B22:C22"/>
+    <mergeCell ref="C1:E1"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
@@ -6097,8 +6097,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6297,11 +6297,11 @@
     <row r="1" spans="2:9" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:9" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="59"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="54"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
@@ -6430,18 +6430,18 @@
       <c r="G10" s="2"/>
     </row>
     <row r="15" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D15" s="77" t="s">
+      <c r="D15" s="64" t="s">
         <v>60</v>
       </c>
-      <c r="E15" s="78"/>
-      <c r="F15" s="78"/>
-      <c r="G15" s="78"/>
+      <c r="E15" s="65"/>
+      <c r="F15" s="65"/>
+      <c r="G15" s="65"/>
     </row>
     <row r="16" spans="2:9" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D16" s="77"/>
-      <c r="E16" s="78"/>
-      <c r="F16" s="78"/>
-      <c r="G16" s="78"/>
+      <c r="D16" s="64"/>
+      <c r="E16" s="65"/>
+      <c r="F16" s="65"/>
+      <c r="G16" s="65"/>
       <c r="H16" t="s">
         <v>70</v>
       </c>
@@ -6451,15 +6451,15 @@
     </row>
     <row r="17" spans="3:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="3:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C18" s="63" t="s">
+      <c r="C18" s="80" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="64"/>
-      <c r="E18" s="65"/>
-      <c r="F18" s="66" t="s">
+      <c r="D18" s="81"/>
+      <c r="E18" s="82"/>
+      <c r="F18" s="83" t="s">
         <v>61</v>
       </c>
-      <c r="G18" s="67"/>
+      <c r="G18" s="84"/>
       <c r="H18" s="48" t="s">
         <v>1</v>
       </c>
@@ -6474,15 +6474,15 @@
       </c>
     </row>
     <row r="19" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C19" s="68" t="s">
+      <c r="C19" s="85" t="s">
         <v>93</v>
       </c>
-      <c r="D19" s="69"/>
-      <c r="E19" s="70"/>
-      <c r="F19" s="74" t="s">
+      <c r="D19" s="86"/>
+      <c r="E19" s="87"/>
+      <c r="F19" s="88" t="s">
         <v>66</v>
       </c>
-      <c r="G19" s="74"/>
+      <c r="G19" s="88"/>
       <c r="H19" s="50">
         <v>2</v>
       </c>
@@ -6497,13 +6497,13 @@
       </c>
     </row>
     <row r="20" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C20" s="71"/>
-      <c r="D20" s="72"/>
-      <c r="E20" s="73"/>
-      <c r="F20" s="62" t="s">
+      <c r="C20" s="69"/>
+      <c r="D20" s="70"/>
+      <c r="E20" s="71"/>
+      <c r="F20" s="77" t="s">
         <v>67</v>
       </c>
-      <c r="G20" s="62"/>
+      <c r="G20" s="77"/>
       <c r="H20" s="36">
         <v>4</v>
       </c>
@@ -6518,15 +6518,15 @@
       </c>
     </row>
     <row r="21" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C21" s="85" t="s">
+      <c r="C21" s="75" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="86"/>
-      <c r="E21" s="86"/>
-      <c r="F21" s="62" t="s">
+      <c r="D21" s="76"/>
+      <c r="E21" s="76"/>
+      <c r="F21" s="77" t="s">
         <v>69</v>
       </c>
-      <c r="G21" s="62"/>
+      <c r="G21" s="77"/>
       <c r="H21" s="36">
         <v>1</v>
       </c>
@@ -6541,13 +6541,13 @@
       </c>
     </row>
     <row r="22" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C22" s="85"/>
-      <c r="D22" s="86"/>
-      <c r="E22" s="86"/>
-      <c r="F22" s="62" t="s">
+      <c r="C22" s="75"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="76"/>
+      <c r="F22" s="77" t="s">
         <v>68</v>
       </c>
-      <c r="G22" s="62"/>
+      <c r="G22" s="77"/>
       <c r="H22" s="36">
         <v>2</v>
       </c>
@@ -6562,9 +6562,9 @@
       </c>
     </row>
     <row r="23" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C23" s="85"/>
-      <c r="D23" s="86"/>
-      <c r="E23" s="86"/>
+      <c r="C23" s="75"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="76"/>
       <c r="F23" s="47" t="s">
         <v>75</v>
       </c>
@@ -6583,81 +6583,81 @@
       </c>
     </row>
     <row r="24" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C24" s="79" t="s">
+      <c r="C24" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="D24" s="80"/>
-      <c r="E24" s="81"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="68"/>
+      <c r="F24" s="77"/>
+      <c r="G24" s="77"/>
       <c r="H24" s="36"/>
       <c r="I24" s="36"/>
       <c r="J24" s="36"/>
       <c r="K24" s="37"/>
     </row>
     <row r="25" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C25" s="71"/>
-      <c r="D25" s="72"/>
-      <c r="E25" s="73"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
+      <c r="C25" s="69"/>
+      <c r="D25" s="70"/>
+      <c r="E25" s="71"/>
+      <c r="F25" s="77"/>
+      <c r="G25" s="77"/>
       <c r="H25" s="36"/>
       <c r="I25" s="36"/>
       <c r="J25" s="36"/>
       <c r="K25" s="37"/>
     </row>
     <row r="26" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C26" s="82"/>
-      <c r="D26" s="83"/>
-      <c r="E26" s="84"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
+      <c r="C26" s="72"/>
+      <c r="D26" s="73"/>
+      <c r="E26" s="74"/>
+      <c r="F26" s="77"/>
+      <c r="G26" s="77"/>
       <c r="H26" s="36"/>
       <c r="I26" s="36"/>
       <c r="J26" s="36"/>
       <c r="K26" s="37"/>
     </row>
     <row r="27" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C27" s="85"/>
-      <c r="D27" s="86"/>
-      <c r="E27" s="86"/>
-      <c r="F27" s="62"/>
-      <c r="G27" s="62"/>
+      <c r="C27" s="75"/>
+      <c r="D27" s="76"/>
+      <c r="E27" s="76"/>
+      <c r="F27" s="77"/>
+      <c r="G27" s="77"/>
       <c r="H27" s="36"/>
       <c r="I27" s="36"/>
       <c r="J27" s="36"/>
       <c r="K27" s="37"/>
     </row>
     <row r="28" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C28" s="85"/>
-      <c r="D28" s="86"/>
-      <c r="E28" s="86"/>
-      <c r="F28" s="62"/>
-      <c r="G28" s="62"/>
+      <c r="C28" s="75"/>
+      <c r="D28" s="76"/>
+      <c r="E28" s="76"/>
+      <c r="F28" s="77"/>
+      <c r="G28" s="77"/>
       <c r="H28" s="36"/>
       <c r="I28" s="36"/>
       <c r="J28" s="36"/>
       <c r="K28" s="37"/>
     </row>
     <row r="29" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C29" s="85"/>
-      <c r="D29" s="86"/>
-      <c r="E29" s="86"/>
-      <c r="F29" s="62"/>
-      <c r="G29" s="62"/>
+      <c r="C29" s="75"/>
+      <c r="D29" s="76"/>
+      <c r="E29" s="76"/>
+      <c r="F29" s="77"/>
+      <c r="G29" s="77"/>
       <c r="H29" s="36"/>
       <c r="I29" s="36"/>
       <c r="J29" s="36"/>
       <c r="K29" s="37"/>
     </row>
     <row r="30" spans="3:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="C30" s="87" t="s">
+      <c r="C30" s="78" t="s">
         <v>19</v>
       </c>
-      <c r="D30" s="88"/>
-      <c r="E30" s="88"/>
-      <c r="F30" s="88"/>
-      <c r="G30" s="88"/>
+      <c r="D30" s="79"/>
+      <c r="E30" s="79"/>
+      <c r="F30" s="79"/>
+      <c r="G30" s="79"/>
       <c r="H30" s="38">
         <f>SUM(H19:H29)</f>
         <v>11</v>
@@ -6676,13 +6676,13 @@
       </c>
     </row>
     <row r="31" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="75" t="s">
+      <c r="C31" s="62" t="s">
         <v>20</v>
       </c>
-      <c r="D31" s="76"/>
-      <c r="E31" s="76"/>
-      <c r="F31" s="76"/>
-      <c r="G31" s="76"/>
+      <c r="D31" s="63"/>
+      <c r="E31" s="63"/>
+      <c r="F31" s="63"/>
+      <c r="G31" s="63"/>
       <c r="H31" s="40">
         <f>SUM(H19:H29)</f>
         <v>11</v>
@@ -6702,6 +6702,14 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="F22:G22"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="F18:G18"/>
+    <mergeCell ref="C19:E20"/>
+    <mergeCell ref="F19:G19"/>
+    <mergeCell ref="F20:G20"/>
     <mergeCell ref="C31:G31"/>
     <mergeCell ref="D15:G16"/>
     <mergeCell ref="C24:E26"/>
@@ -6716,14 +6724,6 @@
     <mergeCell ref="F27:G27"/>
     <mergeCell ref="C21:E23"/>
     <mergeCell ref="F21:G21"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="F22:G22"/>
-    <mergeCell ref="F24:G24"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="F18:G18"/>
-    <mergeCell ref="C19:E20"/>
-    <mergeCell ref="F19:G19"/>
-    <mergeCell ref="F20:G20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -6735,7 +6735,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
@@ -6751,11 +6751,11 @@
     <row r="1" spans="2:8" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="59"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="54"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
@@ -6884,16 +6884,16 @@
       <c r="G10" s="2"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="91" t="s">
+      <c r="C15" s="104" t="s">
         <v>100</v>
       </c>
-      <c r="D15" s="92"/>
-      <c r="E15" s="93"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="106"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="94"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="96"/>
+      <c r="C16" s="107"/>
+      <c r="D16" s="108"/>
+      <c r="E16" s="109"/>
       <c r="G16" t="s">
         <v>70</v>
       </c>
@@ -6903,15 +6903,15 @@
     </row>
     <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="97" t="s">
+      <c r="B18" s="110" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="98"/>
-      <c r="D18" s="99"/>
-      <c r="E18" s="100" t="s">
+      <c r="C18" s="111"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="113" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="101"/>
+      <c r="F18" s="114"/>
       <c r="G18" s="42" t="s">
         <v>1</v>
       </c>
@@ -6926,15 +6926,15 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="79" t="s">
+      <c r="B19" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="C19" s="80"/>
-      <c r="D19" s="108"/>
-      <c r="E19" s="89" t="s">
+      <c r="C19" s="67"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="101" t="s">
         <v>77</v>
       </c>
-      <c r="F19" s="90"/>
+      <c r="F19" s="102"/>
       <c r="G19" s="34"/>
       <c r="H19" s="34">
         <v>0</v>
@@ -6945,13 +6945,13 @@
       <c r="J19" s="35"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="71"/>
-      <c r="C20" s="72"/>
-      <c r="D20" s="109"/>
-      <c r="E20" s="89" t="s">
+      <c r="B20" s="69"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="101" t="s">
         <v>78</v>
       </c>
-      <c r="F20" s="90"/>
+      <c r="F20" s="102"/>
       <c r="G20" s="34">
         <v>4</v>
       </c>
@@ -6966,13 +6966,13 @@
       </c>
     </row>
     <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="71"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="109"/>
-      <c r="E21" s="89" t="s">
+      <c r="B21" s="69"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="96"/>
+      <c r="E21" s="101" t="s">
         <v>79</v>
       </c>
-      <c r="F21" s="90"/>
+      <c r="F21" s="102"/>
       <c r="G21" s="34">
         <v>8</v>
       </c>
@@ -6987,13 +6987,13 @@
       </c>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="71"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="109"/>
-      <c r="E22" s="89" t="s">
+      <c r="B22" s="69"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="96"/>
+      <c r="E22" s="101" t="s">
         <v>80</v>
       </c>
-      <c r="F22" s="90"/>
+      <c r="F22" s="102"/>
       <c r="G22" s="34">
         <v>20</v>
       </c>
@@ -7008,13 +7008,13 @@
       </c>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="82"/>
-      <c r="C23" s="83"/>
-      <c r="D23" s="110"/>
-      <c r="E23" s="89" t="s">
+      <c r="B23" s="72"/>
+      <c r="C23" s="73"/>
+      <c r="D23" s="97"/>
+      <c r="E23" s="101" t="s">
         <v>81</v>
       </c>
-      <c r="F23" s="90"/>
+      <c r="F23" s="102"/>
       <c r="G23" s="34"/>
       <c r="H23" s="34">
         <v>0</v>
@@ -7025,11 +7025,11 @@
       <c r="J23" s="35"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="79" t="s">
+      <c r="B24" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="C24" s="80"/>
-      <c r="D24" s="108"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="95"/>
       <c r="E24" s="45" t="s">
         <v>82</v>
       </c>
@@ -7048,9 +7048,9 @@
       </c>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="82"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="110"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="97"/>
       <c r="E25" s="45" t="s">
         <v>76</v>
       </c>
@@ -7069,79 +7069,79 @@
       </c>
     </row>
     <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="111"/>
-      <c r="C26" s="112"/>
-      <c r="D26" s="113"/>
-      <c r="E26" s="89"/>
-      <c r="F26" s="90"/>
+      <c r="B26" s="98"/>
+      <c r="C26" s="99"/>
+      <c r="D26" s="100"/>
+      <c r="E26" s="101"/>
+      <c r="F26" s="102"/>
       <c r="G26" s="34"/>
       <c r="H26" s="34"/>
       <c r="I26" s="34"/>
       <c r="J26" s="35"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="111"/>
-      <c r="C27" s="112"/>
-      <c r="D27" s="113"/>
-      <c r="E27" s="89"/>
-      <c r="F27" s="90"/>
+      <c r="B27" s="98"/>
+      <c r="C27" s="99"/>
+      <c r="D27" s="100"/>
+      <c r="E27" s="101"/>
+      <c r="F27" s="102"/>
       <c r="G27" s="34"/>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
       <c r="J27" s="35"/>
     </row>
     <row r="28" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="111"/>
-      <c r="C28" s="112"/>
-      <c r="D28" s="113"/>
-      <c r="E28" s="89"/>
-      <c r="F28" s="90"/>
+      <c r="B28" s="98"/>
+      <c r="C28" s="99"/>
+      <c r="D28" s="100"/>
+      <c r="E28" s="101"/>
+      <c r="F28" s="102"/>
       <c r="G28" s="34"/>
       <c r="H28" s="34"/>
       <c r="I28" s="34"/>
       <c r="J28" s="35"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="111"/>
-      <c r="C29" s="112"/>
-      <c r="D29" s="113"/>
-      <c r="E29" s="89"/>
-      <c r="F29" s="90"/>
+      <c r="B29" s="98"/>
+      <c r="C29" s="99"/>
+      <c r="D29" s="100"/>
+      <c r="E29" s="101"/>
+      <c r="F29" s="102"/>
       <c r="G29" s="34"/>
       <c r="H29" s="34"/>
       <c r="I29" s="34"/>
       <c r="J29" s="35"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="85"/>
-      <c r="C30" s="86"/>
-      <c r="D30" s="114"/>
-      <c r="E30" s="89"/>
-      <c r="F30" s="90"/>
+      <c r="B30" s="75"/>
+      <c r="C30" s="76"/>
+      <c r="D30" s="103"/>
+      <c r="E30" s="101"/>
+      <c r="F30" s="102"/>
       <c r="G30" s="34"/>
       <c r="H30" s="34"/>
       <c r="I30" s="34"/>
       <c r="J30" s="35"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="85"/>
-      <c r="C31" s="86"/>
-      <c r="D31" s="114"/>
-      <c r="E31" s="89"/>
-      <c r="F31" s="90"/>
+      <c r="B31" s="75"/>
+      <c r="C31" s="76"/>
+      <c r="D31" s="103"/>
+      <c r="E31" s="101"/>
+      <c r="F31" s="102"/>
       <c r="G31" s="34"/>
       <c r="H31" s="34"/>
       <c r="I31" s="34"/>
       <c r="J31" s="35"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="102" t="s">
+      <c r="B32" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="C32" s="103"/>
-      <c r="D32" s="103"/>
-      <c r="E32" s="103"/>
-      <c r="F32" s="104"/>
+      <c r="C32" s="90"/>
+      <c r="D32" s="90"/>
+      <c r="E32" s="90"/>
+      <c r="F32" s="91"/>
       <c r="G32" s="38">
         <f>SUM(G19:G31)</f>
         <v>38</v>
@@ -7160,13 +7160,13 @@
       </c>
     </row>
     <row r="33" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="105" t="s">
+      <c r="B33" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="C33" s="106"/>
-      <c r="D33" s="106"/>
-      <c r="E33" s="106"/>
-      <c r="F33" s="107"/>
+      <c r="C33" s="93"/>
+      <c r="D33" s="93"/>
+      <c r="E33" s="93"/>
+      <c r="F33" s="94"/>
       <c r="G33" s="40">
         <f>SUM(G19:G31)</f>
         <v>38</v>
@@ -7186,6 +7186,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="E23:F23"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C15:E16"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="E20:F20"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E22:F22"/>
     <mergeCell ref="B32:F32"/>
     <mergeCell ref="B33:F33"/>
     <mergeCell ref="B19:D23"/>
@@ -7202,15 +7211,6 @@
     <mergeCell ref="E27:F27"/>
     <mergeCell ref="B28:D28"/>
     <mergeCell ref="E28:F28"/>
-    <mergeCell ref="E23:F23"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C15:E16"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="E20:F20"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E22:F22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
@@ -7222,8 +7222,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J36"/>
   <sheetViews>
-    <sheetView topLeftCell="A25" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:D28"/>
+    <sheetView topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7238,11 +7238,11 @@
     <row r="1" spans="2:8" ht="54.95" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="2:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
-      <c r="C3" s="57" t="s">
+      <c r="C3" s="52" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="58"/>
-      <c r="E3" s="59"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="54"/>
       <c r="F3" s="2"/>
       <c r="G3" s="2"/>
     </row>
@@ -7305,12 +7305,18 @@
       <c r="B8" s="33" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="7"/>
+      <c r="C8" s="6">
+        <v>6</v>
+      </c>
+      <c r="D8" s="6">
+        <v>6</v>
+      </c>
+      <c r="E8" s="7">
+        <v>6</v>
+      </c>
       <c r="F8" s="11">
         <f>SUM(C8:E8)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="G8" s="2"/>
     </row>
@@ -7320,15 +7326,15 @@
       </c>
       <c r="C9" s="13">
         <f>SUM(C5:C8)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D9" s="13">
         <f>SUM(D5:D8)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="E9" s="14">
         <f>SUM(E5:E8)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="F9" s="2"/>
       <c r="G9" s="2"/>
@@ -7339,7 +7345,7 @@
       </c>
       <c r="C10" s="16">
         <f>SUM(C9+D9+E9)</f>
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
@@ -7347,16 +7353,16 @@
       <c r="G10" s="2"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C15" s="91" t="s">
+      <c r="C15" s="104" t="s">
         <v>60</v>
       </c>
-      <c r="D15" s="92"/>
-      <c r="E15" s="93"/>
+      <c r="D15" s="105"/>
+      <c r="E15" s="106"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="C16" s="94"/>
-      <c r="D16" s="95"/>
-      <c r="E16" s="96"/>
+      <c r="C16" s="107"/>
+      <c r="D16" s="108"/>
+      <c r="E16" s="109"/>
       <c r="G16" t="s">
         <v>70</v>
       </c>
@@ -7366,15 +7372,15 @@
     </row>
     <row r="17" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="18" spans="2:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="97" t="s">
+      <c r="B18" s="110" t="s">
         <v>62</v>
       </c>
-      <c r="C18" s="98"/>
-      <c r="D18" s="99"/>
-      <c r="E18" s="100" t="s">
+      <c r="C18" s="111"/>
+      <c r="D18" s="112"/>
+      <c r="E18" s="113" t="s">
         <v>61</v>
       </c>
-      <c r="F18" s="101"/>
+      <c r="F18" s="114"/>
       <c r="G18" s="42" t="s">
         <v>1</v>
       </c>
@@ -7389,24 +7395,26 @@
       </c>
     </row>
     <row r="19" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B19" s="79" t="s">
+      <c r="B19" s="66" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="80"/>
-      <c r="D19" s="108"/>
-      <c r="E19" s="89" t="s">
+      <c r="C19" s="67"/>
+      <c r="D19" s="95"/>
+      <c r="E19" s="101" t="s">
         <v>84</v>
       </c>
-      <c r="F19" s="90"/>
-      <c r="G19" s="34"/>
+      <c r="F19" s="102"/>
+      <c r="G19" s="34">
+        <v>2</v>
+      </c>
       <c r="H19" s="34"/>
       <c r="I19" s="34"/>
       <c r="J19" s="35"/>
     </row>
     <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B20" s="71"/>
-      <c r="C20" s="72"/>
-      <c r="D20" s="109"/>
+      <c r="B20" s="69"/>
+      <c r="C20" s="70"/>
+      <c r="D20" s="96"/>
       <c r="E20" s="45" t="s">
         <v>87</v>
       </c>
@@ -7417,9 +7425,9 @@
       <c r="J20" s="35"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B21" s="71"/>
-      <c r="C21" s="72"/>
-      <c r="D21" s="109"/>
+      <c r="B21" s="69"/>
+      <c r="C21" s="70"/>
+      <c r="D21" s="96"/>
       <c r="E21" s="45" t="s">
         <v>88</v>
       </c>
@@ -7430,9 +7438,9 @@
       <c r="J21" s="35"/>
     </row>
     <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B22" s="71"/>
-      <c r="C22" s="72"/>
-      <c r="D22" s="109"/>
+      <c r="B22" s="69"/>
+      <c r="C22" s="70"/>
+      <c r="D22" s="96"/>
       <c r="E22" s="45" t="s">
         <v>89</v>
       </c>
@@ -7443,9 +7451,9 @@
       <c r="J22" s="35"/>
     </row>
     <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B23" s="71"/>
-      <c r="C23" s="72"/>
-      <c r="D23" s="109"/>
+      <c r="B23" s="69"/>
+      <c r="C23" s="70"/>
+      <c r="D23" s="96"/>
       <c r="E23" s="45" t="s">
         <v>90</v>
       </c>
@@ -7456,9 +7464,9 @@
       <c r="J23" s="35"/>
     </row>
     <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="71"/>
-      <c r="C24" s="72"/>
-      <c r="D24" s="109"/>
+      <c r="B24" s="69"/>
+      <c r="C24" s="70"/>
+      <c r="D24" s="96"/>
       <c r="E24" s="45" t="s">
         <v>91</v>
       </c>
@@ -7469,9 +7477,9 @@
       <c r="J24" s="35"/>
     </row>
     <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B25" s="82"/>
-      <c r="C25" s="83"/>
-      <c r="D25" s="110"/>
+      <c r="B25" s="72"/>
+      <c r="C25" s="73"/>
+      <c r="D25" s="97"/>
       <c r="E25" s="45" t="s">
         <v>92</v>
       </c>
@@ -7482,133 +7490,137 @@
       <c r="J25" s="35"/>
     </row>
     <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B26" s="111" t="s">
+      <c r="B26" s="98" t="s">
         <v>97</v>
       </c>
-      <c r="C26" s="112"/>
-      <c r="D26" s="113"/>
-      <c r="E26" s="89" t="s">
+      <c r="C26" s="99"/>
+      <c r="D26" s="100"/>
+      <c r="E26" s="101" t="s">
         <v>83</v>
       </c>
-      <c r="F26" s="90"/>
-      <c r="G26" s="34"/>
+      <c r="F26" s="102"/>
+      <c r="G26" s="34">
+        <v>3</v>
+      </c>
       <c r="H26" s="34"/>
       <c r="I26" s="34"/>
       <c r="J26" s="35"/>
     </row>
     <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B27" s="79" t="s">
+      <c r="B27" s="66" t="s">
         <v>98</v>
       </c>
-      <c r="C27" s="80"/>
-      <c r="D27" s="108"/>
-      <c r="E27" s="89" t="s">
+      <c r="C27" s="67"/>
+      <c r="D27" s="95"/>
+      <c r="E27" s="101" t="s">
         <v>85</v>
       </c>
-      <c r="F27" s="90"/>
-      <c r="G27" s="34"/>
+      <c r="F27" s="102"/>
+      <c r="G27" s="34">
+        <v>3</v>
+      </c>
       <c r="H27" s="34"/>
       <c r="I27" s="34"/>
       <c r="J27" s="35"/>
     </row>
     <row r="28" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B28" s="82"/>
-      <c r="C28" s="83"/>
-      <c r="D28" s="110"/>
-      <c r="E28" s="89" t="s">
+      <c r="B28" s="72"/>
+      <c r="C28" s="73"/>
+      <c r="D28" s="97"/>
+      <c r="E28" s="101" t="s">
         <v>86</v>
       </c>
-      <c r="F28" s="90"/>
+      <c r="F28" s="102"/>
       <c r="G28" s="34"/>
       <c r="H28" s="34"/>
       <c r="I28" s="34"/>
       <c r="J28" s="35"/>
     </row>
     <row r="29" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B29" s="111"/>
-      <c r="C29" s="112"/>
-      <c r="D29" s="113"/>
-      <c r="E29" s="89"/>
-      <c r="F29" s="90"/>
+      <c r="B29" s="98"/>
+      <c r="C29" s="99"/>
+      <c r="D29" s="100"/>
+      <c r="E29" s="101"/>
+      <c r="F29" s="102"/>
       <c r="G29" s="34"/>
       <c r="H29" s="34"/>
       <c r="I29" s="34"/>
       <c r="J29" s="35"/>
     </row>
     <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B30" s="111"/>
-      <c r="C30" s="112"/>
-      <c r="D30" s="113"/>
-      <c r="E30" s="89"/>
-      <c r="F30" s="90"/>
+      <c r="B30" s="98"/>
+      <c r="C30" s="99"/>
+      <c r="D30" s="100"/>
+      <c r="E30" s="101"/>
+      <c r="F30" s="102"/>
       <c r="G30" s="34"/>
       <c r="H30" s="34"/>
       <c r="I30" s="34"/>
       <c r="J30" s="35"/>
     </row>
     <row r="31" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B31" s="111"/>
-      <c r="C31" s="112"/>
-      <c r="D31" s="113"/>
-      <c r="E31" s="89"/>
-      <c r="F31" s="90"/>
+      <c r="B31" s="98"/>
+      <c r="C31" s="99"/>
+      <c r="D31" s="100"/>
+      <c r="E31" s="101"/>
+      <c r="F31" s="102"/>
       <c r="G31" s="34"/>
       <c r="H31" s="34"/>
       <c r="I31" s="34"/>
       <c r="J31" s="35"/>
     </row>
     <row r="32" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B32" s="111"/>
-      <c r="C32" s="112"/>
-      <c r="D32" s="113"/>
-      <c r="E32" s="89"/>
-      <c r="F32" s="90"/>
+      <c r="B32" s="98"/>
+      <c r="C32" s="99"/>
+      <c r="D32" s="100"/>
+      <c r="E32" s="101"/>
+      <c r="F32" s="102"/>
       <c r="G32" s="34"/>
       <c r="H32" s="34"/>
       <c r="I32" s="34"/>
       <c r="J32" s="35"/>
     </row>
     <row r="33" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B33" s="85"/>
-      <c r="C33" s="86"/>
-      <c r="D33" s="114"/>
-      <c r="E33" s="89"/>
-      <c r="F33" s="90"/>
+      <c r="B33" s="75"/>
+      <c r="C33" s="76"/>
+      <c r="D33" s="103"/>
+      <c r="E33" s="101"/>
+      <c r="F33" s="102"/>
       <c r="G33" s="34"/>
       <c r="H33" s="34"/>
       <c r="I33" s="34"/>
       <c r="J33" s="35"/>
     </row>
     <row r="34" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B34" s="85"/>
-      <c r="C34" s="86"/>
-      <c r="D34" s="114"/>
-      <c r="E34" s="89"/>
-      <c r="F34" s="90"/>
+      <c r="B34" s="75"/>
+      <c r="C34" s="76"/>
+      <c r="D34" s="103"/>
+      <c r="E34" s="101"/>
+      <c r="F34" s="102"/>
       <c r="G34" s="34"/>
       <c r="H34" s="34"/>
       <c r="I34" s="34"/>
       <c r="J34" s="35"/>
     </row>
     <row r="35" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B35" s="102" t="s">
+      <c r="B35" s="89" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="103"/>
-      <c r="D35" s="103"/>
-      <c r="E35" s="103"/>
-      <c r="F35" s="104"/>
+      <c r="C35" s="90"/>
+      <c r="D35" s="90"/>
+      <c r="E35" s="90"/>
+      <c r="F35" s="91"/>
       <c r="G35" s="38">
         <f>SUM(G19:G34)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H35" s="38">
         <f>G35-(G35/H16)</f>
-        <v>0</v>
+        <v>5.3333333333333339</v>
       </c>
       <c r="I35" s="38">
         <f>G35-2*(G35/H16)</f>
-        <v>0</v>
+        <v>2.666666666666667</v>
       </c>
       <c r="J35" s="39">
         <f>G35-3*(G35/H16)</f>
@@ -7616,32 +7628,41 @@
       </c>
     </row>
     <row r="36" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B36" s="105" t="s">
+      <c r="B36" s="92" t="s">
         <v>20</v>
       </c>
-      <c r="C36" s="106"/>
-      <c r="D36" s="106"/>
-      <c r="E36" s="106"/>
-      <c r="F36" s="107"/>
+      <c r="C36" s="93"/>
+      <c r="D36" s="93"/>
+      <c r="E36" s="93"/>
+      <c r="F36" s="94"/>
       <c r="G36" s="40">
         <f>SUM(G19:G34)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="H36" s="40">
         <f>G36-SUM(H19:H34)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="I36" s="40">
         <f>G36-SUM(H19:I34)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="J36" s="41">
         <f>G36-SUM(H19:J34)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B26:D26"/>
+    <mergeCell ref="E26:F26"/>
+    <mergeCell ref="E27:F27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="C3:E3"/>
+    <mergeCell ref="C15:E16"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="E18:F18"/>
+    <mergeCell ref="E19:F19"/>
     <mergeCell ref="B35:F35"/>
     <mergeCell ref="B36:F36"/>
     <mergeCell ref="B27:D28"/>
@@ -7658,15 +7679,6 @@
     <mergeCell ref="E30:F30"/>
     <mergeCell ref="B31:D31"/>
     <mergeCell ref="E31:F31"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="E26:F26"/>
-    <mergeCell ref="E27:F27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="C3:E3"/>
-    <mergeCell ref="C15:E16"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="E18:F18"/>
-    <mergeCell ref="E19:F19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>

</xml_diff>